<commit_message>
Update RMSE fit thermal conductivity coefficients 2020-08-22.xlsx
some documentation on that excel file
</commit_message>
<xml_diff>
--- a/experimental corroboration/RMSE fit thermal conductivity coefficients 2020-08-22.xlsx
+++ b/experimental corroboration/RMSE fit thermal conductivity coefficients 2020-08-22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\CASE publishing ICSF and\ICSF Experimental Validation Article\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26BE7499-1E2D-45CA-870F-47104D1DFB78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343C292D-ACAD-4E17-AD5C-C1310A564A79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1913" yWindow="270" windowWidth="10829" windowHeight="7560" xr2:uid="{FACE350A-3AAD-4EE9-B271-DF7960D02B72}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Gc_Receiver = 3.66 * 401 / (2 * (0.003175 + 0.01905)) * (2 * Modelica.Constants.pi * (0.003175 + 0.01905) * 0.01 + 2 * Modelica.Constants.pi * (0.003175 + 0.01905) ^ 2)</t>
   </si>
@@ -137,12 +137,24 @@
   </si>
   <si>
     <t>TUBING-AMBIENT CONDUCTIVITY</t>
+  </si>
+  <si>
+    <t>referring to ICSolar.mo in github</t>
+  </si>
+  <si>
+    <t>What are the receiver and tubing loss to ambient coefficients that we arrived at during RSME regression fitting?</t>
+  </si>
+  <si>
+    <t>done for conf paper 2020-08-22</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -172,8 +184,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9758BF27-A375-48A2-89FB-F887990A2DBF}">
-  <dimension ref="A9:G42"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -500,38 +513,53 @@
     <col min="7" max="7" width="50.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="G9">
         <f xml:space="preserve"> 3.66*401 /(2*(0.003175+0.01905)) *(2*Modelica.Constants.pi *(0.003175 + 0.01905)*0.01 +2*Modelica.Constants.pi*(0.003175 + 0.01905)^2)</f>
         <v>148.58270368860579</v>
       </c>
     </row>
-    <row r="10" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="G10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="G12">
         <v>3.66</v>
       </c>
     </row>
-    <row r="13" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="G13">
         <v>401</v>
       </c>
     </row>
-    <row r="14" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="G14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="G15">
         <v>3.1749999999999999E-3</v>
       </c>
     </row>
-    <row r="16" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="G16">
         <v>1.9050000000000001E-2</v>
       </c>
@@ -721,7 +749,7 @@
       <c r="A41" t="s">
         <v>21</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="1">
         <f>1/((1/E21)+(1/E23))</f>
         <v>1.734362872892993E-2</v>
       </c>
@@ -733,7 +761,7 @@
       <c r="A42" t="s">
         <v>22</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="1">
         <f>1/(D31+D33+D35+D37)</f>
         <v>6.6524032866241242E-2</v>
       </c>
@@ -743,5 +771,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>